<commit_message>
i Promice its final
</commit_message>
<xml_diff>
--- a/user_preferences.xlsx
+++ b/user_preferences.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -613,6 +613,132 @@
         <v>20</v>
       </c>
     </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>140</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>2000</v>
+      </c>
+      <c r="B18">
+        <v>140</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>2000</v>
+      </c>
+      <c r="B19">
+        <v>140</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20">
+        <v>140</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21">
+        <v>140</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>1000</v>
+      </c>
+      <c r="B22">
+        <v>140</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>1000</v>
+      </c>
+      <c r="B23">
+        <v>140</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>1000</v>
+      </c>
+      <c r="B24">
+        <v>140</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>1000</v>
+      </c>
+      <c r="B25">
+        <v>140</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>